<commit_message>
Implement full sheet processing.
</commit_message>
<xml_diff>
--- a/src/collective/excelimportexport/tests/import.xlsx
+++ b/src/collective/excelimportexport/tests/import.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>This sheet is ignored</t>
   </si>
@@ -49,6 +49,21 @@
   </si>
   <si>
     <t>&lt;p&gt;Foo &lt;em&gt;document&lt;/em&gt; text&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>News Item</t>
+  </si>
+  <si>
+    <t>/bar-news-item-title</t>
+  </si>
+  <si>
+    <t>Bar News Item Title</t>
+  </si>
+  <si>
+    <t>bar news item description</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;bar &lt;em&gt;news item&lt;/em&gt; text&lt;/p&gt;</t>
   </si>
 </sst>
 </file>
@@ -177,10 +192,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -227,6 +242,23 @@
         <v>10</v>
       </c>
     </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Add coverage for handling lines fields such as 'subjects'
</commit_message>
<xml_diff>
--- a/src/collective/excelimportexport/tests/import.xlsx
+++ b/src/collective/excelimportexport/tests/import.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
   <si>
     <t>This sheet is ignored</t>
   </si>
@@ -31,6 +31,9 @@
     <t>description</t>
   </si>
   <si>
+    <t>subjects</t>
+  </si>
+  <si>
     <t>text</t>
   </si>
   <si>
@@ -43,6 +46,10 @@
     <t>Foo document description</t>
   </si>
   <si>
+    <t>Foo
+Bar</t>
+  </si>
+  <si>
     <t>&lt;p&gt;Foo &lt;em&gt;document&lt;/em&gt; text&lt;/p&gt;</t>
   </si>
   <si>
@@ -53,6 +60,10 @@
   </si>
   <si>
     <t>bar news item description</t>
+  </si>
+  <si>
+    <t>Bar
+Qux</t>
   </si>
   <si>
     <t>&lt;p&gt;bar &lt;em&gt;news item&lt;/em&gt; text&lt;/p&gt;</t>
@@ -167,13 +178,17 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -195,6 +210,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
+    <tabColor rgb="00FFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1"/>
@@ -227,12 +243,13 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
+    <tabColor rgb="00FFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="1:3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -240,8 +257,8 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.1581632653061"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.5510204081633"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.4081632653061"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.030612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="14.030612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -257,35 +274,43 @@
       <c r="D1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="AMI1" s="0"/>
+      <c r="E1" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="AMJ1" s="0"/>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="0" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -302,6 +327,7 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
+    <tabColor rgb="00FFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:E3"/>
@@ -324,7 +350,7 @@
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
@@ -333,41 +359,41 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>18</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>